<commit_message>
update pic and linkedin
</commit_message>
<xml_diff>
--- a/hewag1975cv.xlsx
+++ b/hewag1975cv.xlsx
@@ -5,13 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="profession" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="education" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="skills" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">skills!$A$1:$C$5</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -36,7 +39,7 @@
     <t xml:space="preserve">responsibilities</t>
   </si>
   <si>
-    <t xml:space="preserve">07/2021 - 01/2023</t>
+    <t xml:space="preserve">07/2021 – present</t>
   </si>
   <si>
     <t xml:space="preserve">METER AG, now ADDIUM GmbH</t>
@@ -45,13 +48,13 @@
     <t xml:space="preserve">Senior Data Scientist</t>
   </si>
   <si>
+    <t xml:space="preserve">Analyse multi-sensor data to improve crop management</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implementation of physical plant growth model into production code</t>
   </si>
   <si>
-    <t xml:space="preserve">Sensor data integration and analysis for indoor crop management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provision and maintenance of AWS infrastructure (EC2, S3, ECR, IAM) for the Data Science team</t>
+    <t xml:space="preserve">Provision and maintenance of AWS infrastructure for the Data Science team</t>
   </si>
   <si>
     <t xml:space="preserve">01/2014 - 06/2021</t>
@@ -66,10 +69,10 @@
     <t xml:space="preserve">Managing an inter-disciplinary Data Science team of 8 people</t>
   </si>
   <si>
-    <t xml:space="preserve">Driving product innovation through exploration of new IoT data sources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conceptually develop and implement (semi-)automated processes for data production, optimize workflows</t>
+    <t xml:space="preserve">Driving product innovation through exploration and integration of new (IoT) data sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developing and implementing (semi-)automated processes for data production</t>
   </si>
   <si>
     <t xml:space="preserve">09/2006 - 12/2013</t>
@@ -81,7 +84,7 @@
     <t xml:space="preserve">Consulting retailers and manufacturers on spatial business questions (e.g. site planning, target group modeling)</t>
   </si>
   <si>
-    <t xml:space="preserve">Spatial data production and analysis with regards to industry specific business questions </t>
+    <t xml:space="preserve">Modeling spatial demographics (age, income, spendings) on various scales   </t>
   </si>
   <si>
     <t xml:space="preserve">07/2003 - 07/2006</t>
@@ -120,28 +123,37 @@
     <t xml:space="preserve">Thesis: NDVI time series, Fourier transformation</t>
   </si>
   <si>
-    <t xml:space="preserve">Physical geography (major)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geology (minor)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Physics (minor)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expertise</t>
+    <t xml:space="preserve">Physical geography (major), Geology and Physics (minor) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expertise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 15 years</t>
   </si>
   <si>
     <t xml:space="preserve">R</t>
   </si>
   <si>
-    <t xml:space="preserve">Data transformation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data visualization</t>
+    <t xml:space="preserve">(Spatial) Data wrangling, analysis and visualization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package development (functional programming, unit and integration testing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data modeling and machine learning (ensemble methods, linear models, supervised/unsupervised learning)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 3 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R Shiny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Development of Shiny applications, Setting up and hosting of a Shiny server </t>
   </si>
 </sst>
 </file>
@@ -234,7 +246,20 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -244,11 +269,11 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.02"/>
@@ -409,13 +434,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.22"/>
@@ -476,34 +501,6 @@
       </c>
       <c r="D4" s="0" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -522,13 +519,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.22"/>
@@ -536,39 +535,62 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="0" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-    </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1"/>
+      <c r="A5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C5"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -576,5 +598,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>